<commit_message>
Updated ZAF model - 2025-07-29 13:46
</commit_message>
<xml_diff>
--- a/VerveStacks_ZAF/SubRES_Tmpl/SubRES_REZoning_Sol_Win_andHydro.xlsx
+++ b/VerveStacks_ZAF/SubRES_Tmpl/SubRES_REZoning_Sol_Win_andHydro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ZAF\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1D6223-58AE-41A4-9A11-24955081E18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6072861F-6B70-4DF8-9C15-D93F488DB55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="266">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -1472,7 +1472,7 @@
   <dimension ref="B2:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1700,8 +1700,12 @@
         <v>262</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1728,8 +1732,12 @@
         <v>263</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>

</xml_diff>

<commit_message>
Updated ZAF model - 2025-07-30 13:14
</commit_message>
<xml_diff>
--- a/VerveStacks_ZAF/SubRES_Tmpl/SubRES_REZoning_Sol_Win_andHydro.xlsx
+++ b/VerveStacks_ZAF/SubRES_Tmpl/SubRES_REZoning_Sol_Win_andHydro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ZAF\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5C4D9D-4521-40F0-8CBB-02F5A9344661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0A6EF5-1E44-448F-B69B-20C24F5A1DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="misc" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="251">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>TAct</t>
-  </si>
-  <si>
-    <t>PJ</t>
   </si>
   <si>
     <t>GW</t>
@@ -428,6 +425,9 @@
     <t>~FI_T: USD10~FX~ACT_BND</t>
   </si>
   <si>
+    <t>invcost</t>
+  </si>
+  <si>
     <t>process</t>
   </si>
   <si>
@@ -825,6 +825,9 @@
   </si>
   <si>
     <t>New Hydro Potential - South Africa - Step 1</t>
+  </si>
+  <si>
+    <t>PJ</t>
   </si>
   <si>
     <t>EN_Hydro_ZAF-2</t>
@@ -1428,7 +1431,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -1452,10 +1455,10 @@
         <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>2</v>
@@ -1470,7 +1473,7 @@
         <v>5</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P3" s="1">
         <v>2022</v>
@@ -1481,26 +1484,26 @@
     </row>
     <row r="4" spans="2:20">
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
         <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
       </c>
       <c r="J4" s="1" t="str">
         <f>C4</f>
         <v>ElcAgg_Solar</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M4" s="1">
         <v>1</v>
@@ -1514,19 +1517,19 @@
     </row>
     <row r="5" spans="2:20">
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1535,7 +1538,7 @@
         <v>ElcAgg_Wind</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M5" s="1">
         <v>1</v>
@@ -1549,17 +1552,17 @@
     </row>
     <row r="6" spans="2:20">
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -1569,10 +1572,10 @@
         <v>elc_demand</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M6" s="1">
         <v>1</v>
@@ -1584,22 +1587,22 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="T6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="2:20">
       <c r="B7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1610,7 +1613,7 @@
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -1625,24 +1628,24 @@
     </row>
     <row r="8" spans="2:20">
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1657,24 +1660,24 @@
     </row>
     <row r="9" spans="2:20">
       <c r="B9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -1699,7 +1702,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -1724,7 +1727,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -1749,7 +1752,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -1774,7 +1777,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -1799,7 +1802,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -1824,7 +1827,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -1849,7 +1852,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -1868,7 +1871,7 @@
         <v>Trd_electricity import</v>
       </c>
       <c r="L17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P17">
         <v>0</v>
@@ -1883,7 +1886,7 @@
         <v>Trd_electricity export</v>
       </c>
       <c r="K18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P18">
         <v>0</v>
@@ -1901,7 +1904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5417F31-D792-47CD-82F2-E942FCB1F74A}">
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -1912,7 +1915,7 @@
         <v>0</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="14.65" thickTop="1">
@@ -1944,18 +1947,18 @@
         <v>3</v>
       </c>
       <c r="L2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="M2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="N2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>111</v>
@@ -1964,22 +1967,22 @@
         <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
         <v>111</v>
       </c>
       <c r="J3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="L3">
         <v>492.57000000000033</v>
@@ -1993,7 +1996,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>113</v>
@@ -2002,22 +2005,22 @@
         <v>114</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I4" t="s">
         <v>113</v>
       </c>
       <c r="J4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K4" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="L4">
         <v>62.419499999999985</v>
@@ -2031,7 +2034,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>115</v>
@@ -2040,22 +2043,22 @@
         <v>116</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I5" t="s">
         <v>115</v>
       </c>
       <c r="J5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="L5">
         <v>10.829249999999998</v>
@@ -2069,7 +2072,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>117</v>
@@ -2078,22 +2081,22 @@
         <v>118</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I6" t="s">
         <v>117</v>
       </c>
       <c r="J6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K6" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="L6">
         <v>255.52950000000004</v>
@@ -2107,7 +2110,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>119</v>
@@ -2116,22 +2119,22 @@
         <v>120</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I7" t="s">
         <v>119</v>
       </c>
       <c r="J7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K7" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="L7">
         <v>100.26299999999999</v>
@@ -2145,7 +2148,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>121</v>
@@ -2154,22 +2157,22 @@
         <v>122</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I8" t="s">
         <v>121</v>
       </c>
       <c r="J8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K8" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="L8">
         <v>63.020250000000004</v>
@@ -2183,7 +2186,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>123</v>
@@ -2192,22 +2195,22 @@
         <v>124</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I9" t="s">
         <v>123</v>
       </c>
       <c r="J9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K9" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L9">
         <v>1.125E-2</v>
@@ -2221,7 +2224,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>125</v>
@@ -2230,22 +2233,22 @@
         <v>126</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I10" t="s">
         <v>125</v>
       </c>
       <c r="J10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K10" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L10">
         <v>38.216250000000002</v>
@@ -2259,7 +2262,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>127</v>
@@ -2268,22 +2271,22 @@
         <v>128</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I11" t="s">
         <v>127</v>
       </c>
       <c r="J11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K11" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L11">
         <v>37.311</v>
@@ -2297,7 +2300,7 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
         <v>129</v>
@@ -2306,22 +2309,22 @@
         <v>130</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I12" t="s">
         <v>129</v>
       </c>
       <c r="J12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K12" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L12">
         <v>84.534750000000003</v>
@@ -2335,7 +2338,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>131</v>
@@ -2344,22 +2347,22 @@
         <v>132</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I13" t="s">
         <v>131</v>
       </c>
       <c r="J13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K13" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L13">
         <v>1.155</v>
@@ -2373,7 +2376,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
         <v>133</v>
@@ -2382,22 +2385,22 @@
         <v>134</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I14" t="s">
         <v>133</v>
       </c>
       <c r="J14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K14" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L14">
         <v>16.146000000000001</v>
@@ -2411,7 +2414,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
         <v>135</v>
@@ -2420,22 +2423,22 @@
         <v>136</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I15" t="s">
         <v>135</v>
       </c>
       <c r="J15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K15" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L15">
         <v>29.504250000000003</v>
@@ -2449,7 +2452,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
         <v>137</v>
@@ -2458,22 +2461,22 @@
         <v>138</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I16" t="s">
         <v>137</v>
       </c>
       <c r="J16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K16" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L16">
         <v>1.2172499999999999</v>
@@ -2487,7 +2490,7 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
         <v>139</v>
@@ -2496,22 +2499,22 @@
         <v>140</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I17" t="s">
         <v>139</v>
       </c>
       <c r="J17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K17" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L17">
         <v>10.337249999999999</v>
@@ -2525,7 +2528,7 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>141</v>
@@ -2534,22 +2537,22 @@
         <v>142</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I18" t="s">
         <v>141</v>
       </c>
       <c r="J18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K18" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L18">
         <v>39.425249999999998</v>
@@ -2563,7 +2566,7 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>143</v>
@@ -2572,22 +2575,22 @@
         <v>144</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I19" t="s">
         <v>143</v>
       </c>
       <c r="J19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K19" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L19">
         <v>14.602500000000001</v>
@@ -2601,7 +2604,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>145</v>
@@ -2610,22 +2613,22 @@
         <v>146</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I20" t="s">
         <v>145</v>
       </c>
       <c r="J20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K20" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L20">
         <v>6.6179999999999994</v>
@@ -2639,7 +2642,7 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
         <v>147</v>
@@ -2648,22 +2651,22 @@
         <v>148</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I21" t="s">
         <v>147</v>
       </c>
       <c r="J21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K21" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L21">
         <v>20.594250000000002</v>
@@ -2677,7 +2680,7 @@
     </row>
     <row r="22" spans="1:14">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
         <v>149</v>
@@ -2686,22 +2689,22 @@
         <v>150</v>
       </c>
       <c r="D22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I22" t="s">
         <v>149</v>
       </c>
       <c r="J22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K22" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L22">
         <v>8.645249999999999</v>
@@ -2715,7 +2718,7 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
         <v>151</v>
@@ -2724,22 +2727,22 @@
         <v>152</v>
       </c>
       <c r="D23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I23" t="s">
         <v>151</v>
       </c>
       <c r="J23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K23" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L23">
         <v>2.1585000000000001</v>
@@ -2753,7 +2756,7 @@
     </row>
     <row r="24" spans="1:14">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
         <v>153</v>
@@ -2762,22 +2765,22 @@
         <v>154</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I24" t="s">
         <v>153</v>
       </c>
       <c r="J24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K24" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L24">
         <v>7.8465000000000007</v>
@@ -2791,7 +2794,7 @@
     </row>
     <row r="25" spans="1:14">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
         <v>155</v>
@@ -2800,22 +2803,22 @@
         <v>156</v>
       </c>
       <c r="D25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I25" t="s">
         <v>155</v>
       </c>
       <c r="J25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K25" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L25">
         <v>12.156000000000001</v>
@@ -2829,7 +2832,7 @@
     </row>
     <row r="26" spans="1:14">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B26" t="s">
         <v>157</v>
@@ -2838,22 +2841,22 @@
         <v>158</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I26" t="s">
         <v>157</v>
       </c>
       <c r="J26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K26" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L26">
         <v>0.69674999999999998</v>
@@ -2867,7 +2870,7 @@
     </row>
     <row r="27" spans="1:14">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" t="s">
         <v>159</v>
@@ -2876,22 +2879,22 @@
         <v>160</v>
       </c>
       <c r="D27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I27" t="s">
         <v>159</v>
       </c>
       <c r="J27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K27" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L27">
         <v>10.198500000000001</v>
@@ -2905,7 +2908,7 @@
     </row>
     <row r="28" spans="1:14">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28" t="s">
         <v>161</v>
@@ -2914,22 +2917,22 @@
         <v>162</v>
       </c>
       <c r="D28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I28" t="s">
         <v>161</v>
       </c>
       <c r="J28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K28" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L28">
         <v>3.4837500000000006</v>
@@ -2943,7 +2946,7 @@
     </row>
     <row r="29" spans="1:14">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29" t="s">
         <v>163</v>
@@ -2952,22 +2955,22 @@
         <v>164</v>
       </c>
       <c r="D29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I29" t="s">
         <v>163</v>
       </c>
       <c r="J29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K29" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L29">
         <v>2.53125</v>
@@ -2981,7 +2984,7 @@
     </row>
     <row r="30" spans="1:14">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30" t="s">
         <v>165</v>
@@ -2990,22 +2993,22 @@
         <v>166</v>
       </c>
       <c r="D30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I30" t="s">
         <v>165</v>
       </c>
       <c r="J30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K30" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L30">
         <v>1.0874999999999999</v>
@@ -3019,7 +3022,7 @@
     </row>
     <row r="31" spans="1:14">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B31" t="s">
         <v>167</v>
@@ -3028,22 +3031,22 @@
         <v>168</v>
       </c>
       <c r="D31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I31" t="s">
         <v>167</v>
       </c>
       <c r="J31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K31" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L31">
         <v>4.9770000000000003</v>
@@ -3057,7 +3060,7 @@
     </row>
     <row r="32" spans="1:14">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B32" t="s">
         <v>169</v>
@@ -3066,22 +3069,22 @@
         <v>170</v>
       </c>
       <c r="D32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I32" t="s">
         <v>169</v>
       </c>
       <c r="J32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K32" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L32">
         <v>1.29525</v>
@@ -3095,7 +3098,7 @@
     </row>
     <row r="33" spans="1:14">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
         <v>171</v>
@@ -3104,22 +3107,22 @@
         <v>172</v>
       </c>
       <c r="D33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I33" t="s">
         <v>171</v>
       </c>
       <c r="J33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K33" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L33">
         <v>1.4902500000000001</v>
@@ -3133,7 +3136,7 @@
     </row>
     <row r="34" spans="1:14">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B34" t="s">
         <v>173</v>
@@ -3142,22 +3145,22 @@
         <v>174</v>
       </c>
       <c r="D34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I34" t="s">
         <v>173</v>
       </c>
       <c r="J34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K34" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L34">
         <v>0.75149999999999995</v>
@@ -3171,7 +3174,7 @@
     </row>
     <row r="35" spans="1:14">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
         <v>175</v>
@@ -3180,22 +3183,22 @@
         <v>176</v>
       </c>
       <c r="D35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I35" t="s">
         <v>175</v>
       </c>
       <c r="J35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K35" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L35">
         <v>9.2250000000000014</v>
@@ -3209,7 +3212,7 @@
     </row>
     <row r="36" spans="1:14">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B36" t="s">
         <v>177</v>
@@ -3218,22 +3221,22 @@
         <v>178</v>
       </c>
       <c r="D36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I36" t="s">
         <v>177</v>
       </c>
       <c r="J36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K36" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L36">
         <v>5.10975</v>
@@ -3247,7 +3250,7 @@
     </row>
     <row r="37" spans="1:14">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B37" t="s">
         <v>179</v>
@@ -3256,22 +3259,22 @@
         <v>180</v>
       </c>
       <c r="D37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I37" t="s">
         <v>179</v>
       </c>
       <c r="J37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K37" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L37">
         <v>0.23099999999999998</v>
@@ -3285,7 +3288,7 @@
     </row>
     <row r="38" spans="1:14">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B38" t="s">
         <v>181</v>
@@ -3294,22 +3297,22 @@
         <v>182</v>
       </c>
       <c r="D38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I38" t="s">
         <v>181</v>
       </c>
       <c r="J38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K38" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L38">
         <v>0.80474999999999997</v>
@@ -3323,7 +3326,7 @@
     </row>
     <row r="39" spans="1:14">
       <c r="A39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B39" t="s">
         <v>183</v>
@@ -3332,22 +3335,22 @@
         <v>184</v>
       </c>
       <c r="D39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I39" t="s">
         <v>183</v>
       </c>
       <c r="J39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K39" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L39">
         <v>0.80474999999999997</v>
@@ -3361,7 +3364,7 @@
     </row>
     <row r="40" spans="1:14">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B40" t="s">
         <v>185</v>
@@ -3370,22 +3373,22 @@
         <v>186</v>
       </c>
       <c r="D40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I40" t="s">
         <v>185</v>
       </c>
       <c r="J40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K40" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L40">
         <v>2.53125</v>
@@ -3399,7 +3402,7 @@
     </row>
     <row r="41" spans="1:14">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B41" t="s">
         <v>187</v>
@@ -3408,22 +3411,22 @@
         <v>188</v>
       </c>
       <c r="D41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I41" t="s">
         <v>187</v>
       </c>
       <c r="J41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K41" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L41">
         <v>1.71</v>
@@ -3437,7 +3440,7 @@
     </row>
     <row r="42" spans="1:14">
       <c r="A42" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B42" t="s">
         <v>189</v>
@@ -3446,22 +3449,22 @@
         <v>190</v>
       </c>
       <c r="D42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I42" t="s">
         <v>189</v>
       </c>
       <c r="J42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K42" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L42">
         <v>4.2967500000000003</v>
@@ -3475,7 +3478,7 @@
     </row>
     <row r="43" spans="1:14">
       <c r="A43" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B43" t="s">
         <v>191</v>
@@ -3484,22 +3487,22 @@
         <v>192</v>
       </c>
       <c r="D43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I43" t="s">
         <v>191</v>
       </c>
       <c r="J43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K43" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L43">
         <v>0.22650000000000001</v>
@@ -3513,7 +3516,7 @@
     </row>
     <row r="44" spans="1:14">
       <c r="A44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B44" t="s">
         <v>193</v>
@@ -3522,22 +3525,22 @@
         <v>194</v>
       </c>
       <c r="D44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I44" t="s">
         <v>193</v>
       </c>
       <c r="J44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K44" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L44">
         <v>0.36675000000000002</v>
@@ -3551,7 +3554,7 @@
     </row>
     <row r="45" spans="1:14">
       <c r="A45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B45" t="s">
         <v>195</v>
@@ -3560,22 +3563,22 @@
         <v>196</v>
       </c>
       <c r="D45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I45" t="s">
         <v>195</v>
       </c>
       <c r="J45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K45" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L45">
         <v>6.0000000000000001E-3</v>
@@ -3589,7 +3592,7 @@
     </row>
     <row r="46" spans="1:14">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B46" t="s">
         <v>197</v>
@@ -3598,22 +3601,22 @@
         <v>198</v>
       </c>
       <c r="D46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I46" t="s">
         <v>197</v>
       </c>
       <c r="J46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K46" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L46">
         <v>2.1749999999999999E-2</v>
@@ -3627,7 +3630,7 @@
     </row>
     <row r="47" spans="1:14">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B47" t="s">
         <v>199</v>
@@ -3636,22 +3639,22 @@
         <v>200</v>
       </c>
       <c r="D47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F47" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I47" t="s">
         <v>199</v>
       </c>
       <c r="J47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K47" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L47">
         <v>4.2952500000000002</v>
@@ -3665,7 +3668,7 @@
     </row>
     <row r="48" spans="1:14">
       <c r="A48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B48" t="s">
         <v>201</v>
@@ -3674,22 +3677,22 @@
         <v>202</v>
       </c>
       <c r="D48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I48" t="s">
         <v>201</v>
       </c>
       <c r="J48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K48" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L48">
         <v>5.5589999999999993</v>
@@ -3703,7 +3706,7 @@
     </row>
     <row r="49" spans="1:14">
       <c r="A49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B49" t="s">
         <v>203</v>
@@ -3712,22 +3715,22 @@
         <v>204</v>
       </c>
       <c r="D49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I49" t="s">
         <v>203</v>
       </c>
       <c r="J49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K49" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L49">
         <v>4.6657500000000001</v>
@@ -3741,7 +3744,7 @@
     </row>
     <row r="50" spans="1:14">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B50" t="s">
         <v>205</v>
@@ -3750,22 +3753,22 @@
         <v>206</v>
       </c>
       <c r="D50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F50" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I50" t="s">
         <v>205</v>
       </c>
       <c r="J50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K50" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L50">
         <v>5.7134999999999998</v>
@@ -3779,7 +3782,7 @@
     </row>
     <row r="51" spans="1:14">
       <c r="A51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B51" t="s">
         <v>207</v>
@@ -3788,22 +3791,22 @@
         <v>208</v>
       </c>
       <c r="D51" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F51" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I51" t="s">
         <v>207</v>
       </c>
       <c r="J51" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K51" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L51">
         <v>18.515999999999998</v>
@@ -3817,7 +3820,7 @@
     </row>
     <row r="52" spans="1:14">
       <c r="A52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B52" t="s">
         <v>209</v>
@@ -3826,22 +3829,22 @@
         <v>210</v>
       </c>
       <c r="D52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E52" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I52" t="s">
         <v>209</v>
       </c>
       <c r="J52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K52" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L52">
         <v>12.6</v>
@@ -3855,7 +3858,7 @@
     </row>
     <row r="53" spans="1:14">
       <c r="A53" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B53" t="s">
         <v>211</v>
@@ -3864,22 +3867,22 @@
         <v>212</v>
       </c>
       <c r="D53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E53" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F53" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I53" t="s">
         <v>211</v>
       </c>
       <c r="J53" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K53" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L53">
         <v>19.160250000000001</v>
@@ -3893,7 +3896,7 @@
     </row>
     <row r="54" spans="1:14">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B54" t="s">
         <v>213</v>
@@ -3902,22 +3905,22 @@
         <v>214</v>
       </c>
       <c r="D54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E54" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I54" t="s">
         <v>213</v>
       </c>
       <c r="J54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K54" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L54">
         <v>40.881750000000004</v>
@@ -3931,7 +3934,7 @@
     </row>
     <row r="55" spans="1:14">
       <c r="A55" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B55" t="s">
         <v>215</v>
@@ -3940,22 +3943,22 @@
         <v>216</v>
       </c>
       <c r="D55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I55" t="s">
         <v>215</v>
       </c>
       <c r="J55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K55" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L55">
         <v>30.723000000000003</v>
@@ -3969,7 +3972,7 @@
     </row>
     <row r="56" spans="1:14">
       <c r="A56" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B56" t="s">
         <v>217</v>
@@ -3978,22 +3981,22 @@
         <v>218</v>
       </c>
       <c r="D56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E56" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F56" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I56" t="s">
         <v>217</v>
       </c>
       <c r="J56" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K56" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L56">
         <v>46.914749999999991</v>
@@ -4007,7 +4010,7 @@
     </row>
     <row r="57" spans="1:14">
       <c r="A57" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B57" t="s">
         <v>219</v>
@@ -4016,22 +4019,22 @@
         <v>220</v>
       </c>
       <c r="D57" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E57" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F57" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I57" t="s">
         <v>219</v>
       </c>
       <c r="J57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K57" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L57">
         <v>51.669750000000008</v>
@@ -4045,7 +4048,7 @@
     </row>
     <row r="58" spans="1:14">
       <c r="A58" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B58" t="s">
         <v>221</v>
@@ -4054,22 +4057,22 @@
         <v>222</v>
       </c>
       <c r="D58" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E58" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F58" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I58" t="s">
         <v>221</v>
       </c>
       <c r="J58" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K58" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L58">
         <v>68.436749999999989</v>
@@ -4083,7 +4086,7 @@
     </row>
     <row r="59" spans="1:14">
       <c r="A59" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B59" t="s">
         <v>223</v>
@@ -4092,22 +4095,22 @@
         <v>224</v>
       </c>
       <c r="D59" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E59" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F59" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I59" t="s">
         <v>223</v>
       </c>
       <c r="J59" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K59" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L59">
         <v>44.173499999999997</v>
@@ -4121,7 +4124,7 @@
     </row>
     <row r="60" spans="1:14">
       <c r="A60" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B60" t="s">
         <v>225</v>
@@ -4130,22 +4133,22 @@
         <v>226</v>
       </c>
       <c r="D60" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E60" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I60" t="s">
         <v>225</v>
       </c>
       <c r="J60" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K60" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L60">
         <v>109.62449999999998</v>
@@ -4159,7 +4162,7 @@
     </row>
     <row r="61" spans="1:14">
       <c r="A61" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B61" t="s">
         <v>227</v>
@@ -4168,22 +4171,22 @@
         <v>228</v>
       </c>
       <c r="D61" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E61" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F61" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I61" t="s">
         <v>227</v>
       </c>
       <c r="J61" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K61" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L61">
         <v>58.799250000000001</v>
@@ -4197,7 +4200,7 @@
     </row>
     <row r="62" spans="1:14">
       <c r="A62" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B62" t="s">
         <v>229</v>
@@ -4206,22 +4209,22 @@
         <v>230</v>
       </c>
       <c r="D62" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E62" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F62" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I62" t="s">
         <v>229</v>
       </c>
       <c r="J62" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K62" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L62">
         <v>39.048000000000002</v>
@@ -4235,7 +4238,7 @@
     </row>
     <row r="63" spans="1:14">
       <c r="A63" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B63" t="s">
         <v>231</v>
@@ -4244,22 +4247,22 @@
         <v>232</v>
       </c>
       <c r="D63" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E63" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F63" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I63" t="s">
         <v>231</v>
       </c>
       <c r="J63" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K63" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L63">
         <v>43.053750000000001</v>
@@ -4273,7 +4276,7 @@
     </row>
     <row r="64" spans="1:14">
       <c r="A64" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B64" t="s">
         <v>233</v>
@@ -4282,22 +4285,22 @@
         <v>234</v>
       </c>
       <c r="D64" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E64" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F64" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I64" t="s">
         <v>233</v>
       </c>
       <c r="J64" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K64" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L64">
         <v>33.171750000000003</v>
@@ -4311,7 +4314,7 @@
     </row>
     <row r="65" spans="1:14">
       <c r="A65" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B65" t="s">
         <v>235</v>
@@ -4320,22 +4323,22 @@
         <v>236</v>
       </c>
       <c r="D65" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E65" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F65" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I65" t="s">
         <v>235</v>
       </c>
       <c r="J65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K65" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L65">
         <v>21.27825</v>
@@ -4349,7 +4352,7 @@
     </row>
     <row r="66" spans="1:14">
       <c r="A66" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B66" t="s">
         <v>237</v>
@@ -4358,22 +4361,22 @@
         <v>238</v>
       </c>
       <c r="D66" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E66" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F66" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I66" t="s">
         <v>237</v>
       </c>
       <c r="J66" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K66" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L66">
         <v>0.94874999999999998</v>
@@ -4387,7 +4390,7 @@
     </row>
     <row r="67" spans="1:14">
       <c r="A67" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B67" t="s">
         <v>239</v>
@@ -4396,22 +4399,22 @@
         <v>240</v>
       </c>
       <c r="D67" t="s">
-        <v>10</v>
+        <v>241</v>
       </c>
       <c r="E67" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F67" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I67" t="s">
         <v>239</v>
       </c>
       <c r="J67" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K67" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L67">
         <v>0.97599999999999998</v>
@@ -4419,31 +4422,31 @@
     </row>
     <row r="68" spans="1:14">
       <c r="A68" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B68" t="s">
+        <v>242</v>
+      </c>
+      <c r="C68" t="s">
+        <v>243</v>
+      </c>
+      <c r="D68" t="s">
         <v>241</v>
       </c>
-      <c r="C68" t="s">
+      <c r="E68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F68" t="s">
+        <v>15</v>
+      </c>
+      <c r="I68" t="s">
         <v>242</v>
       </c>
-      <c r="D68" t="s">
-        <v>10</v>
-      </c>
-      <c r="E68" t="s">
-        <v>11</v>
-      </c>
-      <c r="F68" t="s">
-        <v>16</v>
-      </c>
-      <c r="I68" t="s">
-        <v>241</v>
-      </c>
       <c r="J68" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K68" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L68">
         <v>0.92300000000000004</v>
@@ -4451,31 +4454,31 @@
     </row>
     <row r="69" spans="1:14">
       <c r="A69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B69" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C69" t="s">
+        <v>245</v>
+      </c>
+      <c r="D69" t="s">
+        <v>241</v>
+      </c>
+      <c r="E69" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" t="s">
+        <v>15</v>
+      </c>
+      <c r="I69" t="s">
         <v>244</v>
       </c>
-      <c r="D69" t="s">
-        <v>10</v>
-      </c>
-      <c r="E69" t="s">
-        <v>11</v>
-      </c>
-      <c r="F69" t="s">
-        <v>16</v>
-      </c>
-      <c r="I69" t="s">
-        <v>243</v>
-      </c>
       <c r="J69" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K69" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L69">
         <v>0.83099999999999996</v>
@@ -4518,7 +4521,7 @@
   <sheetData>
     <row r="2" spans="2:23">
       <c r="B2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -4530,63 +4533,63 @@
     </row>
     <row r="3" spans="2:23">
       <c r="B3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="2:23">
       <c r="B4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="2:23">
       <c r="C5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:23">
@@ -4604,7 +4607,7 @@
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
@@ -4627,29 +4630,29 @@
         <v>7</v>
       </c>
       <c r="E9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="G9" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7" t="s">
         <v>1</v>
       </c>
       <c r="J9" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="K9" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="L9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="N9" s="7">
         <f>J35</f>
@@ -4683,46 +4686,46 @@
         <v>3</v>
       </c>
       <c r="V9" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="W9" t="s">
         <v>62</v>
-      </c>
-      <c r="W9" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="10" spans="2:23">
       <c r="B10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>66</v>
-      </c>
       <c r="E10" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J10" s="7" t="s">
-        <v>68</v>
-      </c>
       <c r="K10" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N10" s="10">
         <f>1/N17</f>
@@ -4746,35 +4749,35 @@
     <row r="11" spans="2:23">
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J11" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="K11" s="7" t="s">
-        <v>71</v>
-      </c>
       <c r="L11" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N11" s="10">
         <f>4/24</f>
@@ -4800,17 +4803,17 @@
       <c r="G12" s="6"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L12" s="7"/>
       <c r="M12" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N12" s="10">
         <v>1</v>
@@ -4833,10 +4836,10 @@
       <c r="G13" s="6"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
@@ -4874,10 +4877,10 @@
     </row>
     <row r="14" spans="2:23">
       <c r="I14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N14" s="4">
         <f>J44</f>
@@ -4910,13 +4913,13 @@
     </row>
     <row r="15" spans="2:23">
       <c r="I15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N15" s="4">
         <v>1</v>
@@ -4930,10 +4933,10 @@
     </row>
     <row r="16" spans="2:23">
       <c r="I16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N16" s="10">
         <v>31.536000000000001</v>
@@ -4947,10 +4950,10 @@
     </row>
     <row r="17" spans="9:23">
       <c r="I17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N17" s="4">
         <v>0.85</v>
@@ -4964,19 +4967,19 @@
     </row>
     <row r="18" spans="9:23">
       <c r="I18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N18" s="10">
         <f>1/N25</f>
@@ -4999,19 +5002,19 @@
     </row>
     <row r="19" spans="9:23">
       <c r="I19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J19" t="s">
+        <v>69</v>
+      </c>
+      <c r="K19" t="s">
         <v>70</v>
       </c>
-      <c r="K19" t="s">
-        <v>71</v>
-      </c>
       <c r="L19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N19" s="4">
         <f>8/24</f>
@@ -5030,16 +5033,16 @@
     </row>
     <row r="20" spans="9:23">
       <c r="I20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N20" s="4">
         <v>1</v>
@@ -5053,10 +5056,10 @@
     </row>
     <row r="21" spans="9:23">
       <c r="I21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N21" s="4">
         <f>J49</f>
@@ -5089,10 +5092,10 @@
     </row>
     <row r="22" spans="9:23">
       <c r="I22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N22" s="4">
         <f>J53</f>
@@ -5125,13 +5128,13 @@
     </row>
     <row r="23" spans="9:23">
       <c r="I23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N23" s="4">
         <v>1</v>
@@ -5145,10 +5148,10 @@
     </row>
     <row r="24" spans="9:23">
       <c r="I24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N24" s="10">
         <v>31.536000000000001</v>
@@ -5162,10 +5165,10 @@
     </row>
     <row r="25" spans="9:23">
       <c r="I25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N25" s="4">
         <v>0.85</v>
@@ -5179,7 +5182,7 @@
     </row>
     <row r="31" spans="9:23" ht="15.75">
       <c r="I31" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
@@ -5191,7 +5194,7 @@
     </row>
     <row r="32" spans="9:23" ht="15.75">
       <c r="I32" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
@@ -5213,7 +5216,7 @@
     </row>
     <row r="34" spans="9:16" ht="15.75">
       <c r="I34" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
@@ -5249,7 +5252,7 @@
     </row>
     <row r="36" spans="9:16" ht="15.75">
       <c r="I36" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J36" s="15"/>
       <c r="K36" s="15"/>
@@ -5261,7 +5264,7 @@
     </row>
     <row r="37" spans="9:16" ht="15.75">
       <c r="I37" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J37" s="15"/>
       <c r="K37" s="15"/>
@@ -5273,7 +5276,7 @@
     </row>
     <row r="38" spans="9:16" ht="15.75">
       <c r="I38" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J38" s="17">
         <v>1363</v>
@@ -5299,7 +5302,7 @@
     </row>
     <row r="39" spans="9:16" ht="15.75">
       <c r="I39" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J39" s="17">
         <v>1363</v>
@@ -5325,7 +5328,7 @@
     </row>
     <row r="40" spans="9:16" ht="15.75">
       <c r="I40" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J40" s="17">
         <v>1363</v>
@@ -5351,7 +5354,7 @@
     </row>
     <row r="41" spans="9:16" ht="15.75">
       <c r="I41" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J41" s="18"/>
       <c r="K41" s="18"/>
@@ -5363,7 +5366,7 @@
     </row>
     <row r="42" spans="9:16" ht="15.75">
       <c r="I42" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J42" s="19">
         <v>34</v>
@@ -5389,7 +5392,7 @@
     </row>
     <row r="43" spans="9:16" ht="15.75">
       <c r="I43" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J43" s="19">
         <v>34</v>
@@ -5415,7 +5418,7 @@
     </row>
     <row r="44" spans="9:16" ht="15.75">
       <c r="I44" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J44" s="19">
         <v>34</v>
@@ -5441,7 +5444,7 @@
     </row>
     <row r="45" spans="9:16" ht="15.75">
       <c r="I45" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J45" s="18"/>
       <c r="K45" s="18"/>
@@ -5453,7 +5456,7 @@
     </row>
     <row r="46" spans="9:16" ht="15.75">
       <c r="I46" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J46" s="18"/>
       <c r="K46" s="18"/>
@@ -5465,7 +5468,7 @@
     </row>
     <row r="47" spans="9:16" ht="15.75">
       <c r="I47" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J47" s="17">
         <v>2470</v>
@@ -5491,7 +5494,7 @@
     </row>
     <row r="48" spans="9:16" ht="15.75">
       <c r="I48" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J48" s="17">
         <v>2470</v>
@@ -5517,7 +5520,7 @@
     </row>
     <row r="49" spans="9:16" ht="15.75">
       <c r="I49" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J49" s="17">
         <v>2470</v>
@@ -5543,7 +5546,7 @@
     </row>
     <row r="50" spans="9:16" ht="15.75">
       <c r="I50" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J50" s="18"/>
       <c r="K50" s="18"/>
@@ -5555,7 +5558,7 @@
     </row>
     <row r="51" spans="9:16" ht="15.75">
       <c r="I51" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J51" s="19">
         <v>62</v>
@@ -5581,7 +5584,7 @@
     </row>
     <row r="52" spans="9:16" ht="15.75">
       <c r="I52" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J52" s="19">
         <v>62</v>
@@ -5607,7 +5610,7 @@
     </row>
     <row r="53" spans="9:16" ht="15.75">
       <c r="I53" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J53" s="19">
         <v>62</v>
@@ -5643,7 +5646,7 @@
     </row>
     <row r="55" spans="9:16" ht="15.75">
       <c r="I55" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J55" s="12">
         <v>0.85</v>
@@ -5657,7 +5660,7 @@
     </row>
     <row r="56" spans="9:16" ht="15.75">
       <c r="I56" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J56" s="12"/>
       <c r="K56" s="12"/>
@@ -5669,7 +5672,7 @@
     </row>
     <row r="57" spans="9:16" ht="15.75">
       <c r="I57" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J57" s="12"/>
       <c r="K57" s="12"/>
@@ -5727,10 +5730,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12EA90E-43F0-4F26-A089-D51219939B11}">
-  <dimension ref="B3:X8"/>
+  <dimension ref="B3:Y8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5747,18 +5750,19 @@
     <col min="11" max="11" width="6.73046875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.796875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.9296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.46484375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.53125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="37.9296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.06640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.3984375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.73046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.9296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.46484375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.53125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="37.9296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.06640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:24">
+    <row r="3" spans="2:25">
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -5766,7 +5770,7 @@
       <c r="F3" s="24"/>
       <c r="G3" s="24"/>
       <c r="H3" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I3" s="24"/>
       <c r="J3" s="24"/>
@@ -5776,18 +5780,19 @@
       <c r="N3" s="24"/>
       <c r="O3" s="24"/>
       <c r="P3" s="24"/>
-      <c r="Q3" s="24" t="s">
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="24"/>
       <c r="S3" s="24"/>
       <c r="T3" s="24"/>
       <c r="U3" s="24"/>
       <c r="V3" s="24"/>
       <c r="W3" s="24"/>
       <c r="X3" s="24"/>
-    </row>
-    <row r="4" spans="2:24">
+      <c r="Y3" s="24"/>
+    </row>
+    <row r="4" spans="2:25">
       <c r="B4" s="24" t="s">
         <v>1</v>
       </c>
@@ -5798,16 +5803,16 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" t="s">
         <v>91</v>
-      </c>
-      <c r="H4" t="s">
-        <v>92</v>
       </c>
       <c r="I4">
         <v>2030</v>
@@ -5816,98 +5821,105 @@
         <v>0</v>
       </c>
       <c r="K4" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="L4" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="M4" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="O4" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="M4" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="N4" s="24" t="s">
+      <c r="P4" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="S4" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="T4" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="U4" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="V4" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="W4" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="X4" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="R4" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="S4" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="T4" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="U4" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="V4" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="W4" s="24" t="s">
+      <c r="Y4" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="X4" s="24" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="2:24">
+    </row>
+    <row r="5" spans="2:25">
       <c r="B5" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K5" s="24">
         <v>0.90249999999999997</v>
       </c>
       <c r="L5" s="26">
+        <f>24/6</f>
         <v>4</v>
       </c>
       <c r="M5" s="24">
         <v>10</v>
       </c>
-      <c r="N5" s="26">
-        <v>3.6</v>
-      </c>
-      <c r="O5" s="24">
+      <c r="N5" s="24">
+        <v>150</v>
+      </c>
+      <c r="O5" s="26">
         <v>1</v>
       </c>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="R5" s="24" t="str">
+      <c r="P5" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="S5" s="24" t="str">
         <f>B5</f>
         <v>EV_Battery</v>
       </c>
-      <c r="S5" s="24" t="s">
-        <v>99</v>
-      </c>
       <c r="T5" s="24" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="U5" s="24" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="V5" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="W5" s="24"/>
+        <v>22</v>
+      </c>
+      <c r="W5" s="24" t="s">
+        <v>15</v>
+      </c>
       <c r="X5" s="24"/>
-    </row>
-    <row r="6" spans="2:24">
+      <c r="Y5" s="24"/>
+    </row>
+    <row r="6" spans="2:25">
       <c r="B6" s="24"/>
       <c r="F6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K6" s="24"/>
       <c r="L6" s="25">
@@ -5925,14 +5937,15 @@
       <c r="V6" s="24"/>
       <c r="W6" s="24"/>
       <c r="X6" s="24"/>
-    </row>
-    <row r="7" spans="2:24">
+      <c r="Y6" s="24"/>
+    </row>
+    <row r="7" spans="2:25">
       <c r="B7" s="24"/>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K7" s="24"/>
       <c r="L7" s="24"/>
@@ -5948,8 +5961,9 @@
       <c r="V7" s="24"/>
       <c r="W7" s="24"/>
       <c r="X7" s="24"/>
-    </row>
-    <row r="8" spans="2:24" ht="17.649999999999999">
+      <c r="Y7" s="24"/>
+    </row>
+    <row r="8" spans="2:25" ht="17.649999999999999">
       <c r="B8" s="21"/>
       <c r="E8" s="27"/>
       <c r="F8" t="str">
@@ -5961,7 +5975,7 @@
         <v>AuxStoIN</v>
       </c>
       <c r="H8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -5974,15 +5988,16 @@
       <c r="M8" s="22"/>
       <c r="N8" s="22"/>
       <c r="O8" s="22"/>
-      <c r="P8" s="21"/>
+      <c r="P8" s="22"/>
       <c r="Q8" s="21"/>
       <c r="R8" s="21"/>
       <c r="S8" s="21"/>
       <c r="T8" s="21"/>
       <c r="U8" s="21"/>
-      <c r="V8" s="23"/>
+      <c r="V8" s="21"/>
       <c r="W8" s="23"/>
       <c r="X8" s="23"/>
+      <c r="Y8" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>